<commit_message>
attacment file and generate ticketnumber
</commit_message>
<xml_diff>
--- a/routes/Requests.xlsx
+++ b/routes/Requests.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>Index</t>
   </si>
@@ -80,36 +80,6 @@
   </si>
   <si>
     <t>2023-08-29T07:28:37.962Z</t>
-  </si>
-  <si>
-    <t>saman_7@gmail.com</t>
-  </si>
-  <si>
-    <t>2023-08-29T07:28:41.344Z</t>
-  </si>
-  <si>
-    <t>saman_8@gmail.com</t>
-  </si>
-  <si>
-    <t>2023-08-29T07:28:45.727Z</t>
-  </si>
-  <si>
-    <t>saman_10@gmail.com</t>
-  </si>
-  <si>
-    <t>2023-08-29T07:28:53.755Z</t>
-  </si>
-  <si>
-    <t>saman_11@gmail.com</t>
-  </si>
-  <si>
-    <t>2023-08-29T07:28:57.177Z</t>
-  </si>
-  <si>
-    <t>saman_13@gmail.com</t>
-  </si>
-  <si>
-    <t>2023-08-29T07:29:04.533Z</t>
   </si>
 </sst>
 </file>
@@ -486,7 +456,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -615,166 +585,6 @@
       </c>
       <c r="J4" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>